<commit_message>
Updated main script with notes to access and store data, formatted the excel log
</commit_message>
<xml_diff>
--- a/Data/Records.xlsx
+++ b/Data/Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohin\Transition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96694D57-3FB6-4110-AEFB-D87D2446C471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E831147-2B03-457D-91BC-CD819A114260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -44,22 +44,28 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Swimming</t>
   </si>
   <si>
     <t>Rest</t>
   </si>
   <si>
-    <t>Gym</t>
-  </si>
-  <si>
     <t>Running</t>
   </si>
   <si>
-    <t>Distance</t>
+    <t>Intensity Rating (1-10)</t>
+  </si>
+  <si>
+    <t>Strength Training - Chest</t>
+  </si>
+  <si>
+    <t>Strength Training - Legs</t>
+  </si>
+  <si>
+    <t>Duration (min)</t>
+  </si>
+  <si>
+    <t>Distance (m)</t>
   </si>
 </sst>
 </file>
@@ -417,21 +423,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ADBCD0-968F-469A-8B27-8E7CAEBDE06E}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I17" sqref="I17:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.47265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1015625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83984375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.83984375" style="1"/>
+    <col min="2" max="2" width="24.20703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.20703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.15625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5234375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,70 +447,103 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>45208</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2" s="1">
+        <v>550</v>
+      </c>
+      <c r="E2" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>45209</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>45210</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>90</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>45211</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>120</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>45212</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="1">
+        <v>650</v>
+      </c>
+      <c r="E6" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>45213</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="1">
+        <v>6470</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>45214</v>
       </c>

</xml_diff>

<commit_message>
Updated records with recent fitness activity
</commit_message>
<xml_diff>
--- a/Data/Records.xlsx
+++ b/Data/Records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohin\Transition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E831147-2B03-457D-91BC-CD819A114260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D163A929-BE50-4FBC-927D-ABF454C9581E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="28992" windowHeight="15672" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -56,24 +56,62 @@
     <t>Intensity Rating (1-10)</t>
   </si>
   <si>
-    <t>Strength Training - Chest</t>
-  </si>
-  <si>
-    <t>Strength Training - Legs</t>
-  </si>
-  <si>
     <t>Duration (min)</t>
   </si>
   <si>
     <t>Distance (m)</t>
+  </si>
+  <si>
+    <t>Gym</t>
+  </si>
+  <si>
+    <t>Time of Day (hh:mm)</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Breatstroke</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Breaststroke</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Easy run</t>
+  </si>
+  <si>
+    <t>Breatstroke / Frontcrawl</t>
+  </si>
+  <si>
+    <t>Breaststroke / Frontcrawl</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,12 +139,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -423,57 +467,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ADBCD0-968F-469A-8B27-8E7CAEBDE06E}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:I18"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.47265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.20703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.20703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.15625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5234375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83984375" style="1"/>
+    <col min="2" max="2" width="13.734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.20703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.20703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.20703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5234375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.20703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>45208</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
         <v>30</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>550</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G2" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>45209</v>
       </c>
@@ -481,74 +543,228 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>45210</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
         <v>90</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G4" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>45211</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1">
+        <v>120</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G5" s="1">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
-        <v>120</v>
-      </c>
-      <c r="E5" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>45212</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
         <v>30</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>650</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G6" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>45213</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1">
         <v>35</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>6470</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="G7" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>45214</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>45215</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1">
+        <v>700</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>45215</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>90</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2">
+        <v>45216</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2">
+        <v>45217</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1">
+        <v>900</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2">
+        <v>45217</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <v>90</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2">
+        <v>45218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2">
+        <v>45219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2">
+        <v>45220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="2">
+        <v>45221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2">
+        <v>45222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2">
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="2">
+        <v>45224</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added and remove files, re-made code strucutre template
</commit_message>
<xml_diff>
--- a/Data/Records.xlsx
+++ b/Data/Records.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohin\Transition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D163A929-BE50-4FBC-927D-ABF454C9581E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F17A2C72-67AA-49C0-AC0B-9DD4A17993AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="28992" windowHeight="15672" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Activity" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -86,16 +86,37 @@
     <t>Back</t>
   </si>
   <si>
-    <t>Easy run</t>
-  </si>
-  <si>
     <t>Breatstroke / Frontcrawl</t>
   </si>
   <si>
     <t>Breaststroke / Frontcrawl</t>
   </si>
   <si>
-    <t>Notes</t>
+    <t>Breastroke / Frontcrawl</t>
+  </si>
+  <si>
+    <t>Short run</t>
+  </si>
+  <si>
+    <t>Legs / Shoulders</t>
+  </si>
+  <si>
+    <t>Body Weight (kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Running </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short run </t>
+  </si>
+  <si>
+    <t>Shoulders / Arms</t>
+  </si>
+  <si>
+    <t>29/10.2023</t>
+  </si>
+  <si>
+    <t>Chest / Triceps</t>
   </si>
 </sst>
 </file>
@@ -467,22 +488,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ADBCD0-968F-469A-8B27-8E7CAEBDE06E}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.47265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.20703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.20703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.20703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.41796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.68359375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.15625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.15625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.15625" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5234375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.20703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
@@ -509,7 +530,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -534,6 +555,9 @@
       <c r="G2" s="1">
         <v>8</v>
       </c>
+      <c r="H2" s="1">
+        <v>74.099999999999994</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
@@ -614,10 +638,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1">
         <v>6470</v>
@@ -645,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1">
         <v>30</v>
@@ -696,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1">
         <v>40</v>
@@ -732,35 +756,328 @@
       <c r="A14" s="2">
         <v>45218</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1">
+        <v>40</v>
+      </c>
+      <c r="E14" s="1">
+        <v>800</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
-        <v>45219</v>
+        <v>45218</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1">
+        <v>90</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G15" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
+        <v>45219</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="2">
         <v>45220</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="2">
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1">
+        <v>34</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6260</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="G17" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2">
         <v>45221</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2">
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="1">
+        <v>90</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2">
         <v>45222</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2">
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1">
+        <v>800</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G19" s="1">
+        <v>6</v>
+      </c>
+      <c r="H19" s="1">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="2">
+        <v>45222</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1">
+        <v>60</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G20" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="2">
         <v>45223</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2">
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="2">
         <v>45224</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1">
+        <v>40</v>
+      </c>
+      <c r="E22" s="1">
+        <v>500</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G22" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <v>30</v>
+      </c>
+      <c r="E23" s="1">
+        <v>700</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="G23" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1">
+        <v>70</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="2">
+        <v>45226</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2">
+        <v>45227</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1">
+        <v>35</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6340</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="G26" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="2">
+        <v>45227</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1">
+        <v>90</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G27" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1">
+        <v>90</v>
+      </c>
+      <c r="G28" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="2">
+        <v>45229</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1">
+        <v>30</v>
+      </c>
+      <c r="E29" s="1">
+        <v>750</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G29" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="2">
+        <v>45229</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="1">
+        <v>80</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G30" s="1">
+        <v>7</v>
+      </c>
+      <c r="H30" s="1">
+        <v>74.900000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated version for data files, need to keep working and update structure for routine
</commit_message>
<xml_diff>
--- a/Data/Records.xlsx
+++ b/Data/Records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohin\Transition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F17A2C72-67AA-49C0-AC0B-9DD4A17993AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346CA747-C75C-4982-9213-C56D3FFD0CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,21 @@
   </si>
   <si>
     <t>Chest / Triceps</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Short Run</t>
+  </si>
+  <si>
+    <t>Shoulders / Triceps</t>
+  </si>
+  <si>
+    <t>Core / Chest</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Abs</t>
   </si>
 </sst>
 </file>
@@ -488,26 +503,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ADBCD0-968F-469A-8B27-8E7CAEBDE06E}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.41796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.68359375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.15625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.15625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.15625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83984375" style="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -533,7 +548,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45208</v>
       </c>
@@ -559,7 +574,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45209</v>
       </c>
@@ -567,7 +582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45210</v>
       </c>
@@ -587,7 +602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45211</v>
       </c>
@@ -607,7 +622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45212</v>
       </c>
@@ -630,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45213</v>
       </c>
@@ -653,7 +668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45214</v>
       </c>
@@ -661,7 +676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45215</v>
       </c>
@@ -684,7 +699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45215</v>
       </c>
@@ -704,7 +719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45216</v>
       </c>
@@ -712,7 +727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45217</v>
       </c>
@@ -735,7 +750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45217</v>
       </c>
@@ -752,7 +767,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45218</v>
       </c>
@@ -775,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45218</v>
       </c>
@@ -795,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45219</v>
       </c>
@@ -803,7 +818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45220</v>
       </c>
@@ -826,7 +841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45221</v>
       </c>
@@ -846,7 +861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45222</v>
       </c>
@@ -872,7 +887,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45222</v>
       </c>
@@ -892,7 +907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45223</v>
       </c>
@@ -900,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45224</v>
       </c>
@@ -923,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45225</v>
       </c>
@@ -946,7 +961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45225</v>
       </c>
@@ -966,7 +981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45226</v>
       </c>
@@ -974,7 +989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45227</v>
       </c>
@@ -997,7 +1012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45227</v>
       </c>
@@ -1017,7 +1032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1034,7 +1049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45229</v>
       </c>
@@ -1057,7 +1072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45229</v>
       </c>
@@ -1078,6 +1093,245 @@
       </c>
       <c r="H30" s="1">
         <v>74.900000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1">
+        <v>30</v>
+      </c>
+      <c r="E31" s="1">
+        <v>525</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="G31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1">
+        <v>90</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G32" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>45231</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>45232</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="1">
+        <v>35</v>
+      </c>
+      <c r="E34" s="1">
+        <v>800</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="G34" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>45233</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>45234</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45</v>
+      </c>
+      <c r="E36" s="1">
+        <v>7150</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.4069444444444445</v>
+      </c>
+      <c r="G36" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>45234</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1">
+        <v>120</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="G37" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>45235</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="1">
+        <v>90</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="G38" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>45236</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1">
+        <v>35</v>
+      </c>
+      <c r="E39" s="1">
+        <v>750</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G39" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>45236</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="1">
+        <v>10</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G40" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>45237</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="1">
+        <v>75</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="G41" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>45238</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1">
+        <v>30</v>
+      </c>
+      <c r="E42" s="1">
+        <v>600</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G42" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>45239</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited data and added seaborn multi-grid plots
</commit_message>
<xml_diff>
--- a/Data/Records.xlsx
+++ b/Data/Records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohin\Transition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346CA747-C75C-4982-9213-C56D3FFD0CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC6405B-ACD5-4D25-A70C-5399C3BE2802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="26910" windowHeight="12990" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -71,30 +71,15 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Breatstroke</t>
-  </si>
-  <si>
     <t>Chest</t>
   </si>
   <si>
     <t>Legs</t>
   </si>
   <si>
-    <t>Breaststroke</t>
-  </si>
-  <si>
     <t>Back</t>
   </si>
   <si>
-    <t>Breatstroke / Frontcrawl</t>
-  </si>
-  <si>
-    <t>Breaststroke / Frontcrawl</t>
-  </si>
-  <si>
-    <t>Breastroke / Frontcrawl</t>
-  </si>
-  <si>
     <t>Short run</t>
   </si>
   <si>
@@ -113,15 +98,9 @@
     <t>Shoulders / Arms</t>
   </si>
   <si>
-    <t>29/10.2023</t>
-  </si>
-  <si>
     <t>Chest / Triceps</t>
   </si>
   <si>
-    <t xml:space="preserve"> Short Run</t>
-  </si>
-  <si>
     <t>Shoulders / Triceps</t>
   </si>
   <si>
@@ -132,22 +111,50 @@
   </si>
   <si>
     <t>Abs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swimming </t>
+  </si>
+  <si>
+    <t>Back / Biceps</t>
+  </si>
+  <si>
+    <t>Football</t>
+  </si>
+  <si>
+    <t>Chest &amp; Shoulders</t>
+  </si>
+  <si>
+    <t>Legs &amp; Calves</t>
+  </si>
+  <si>
+    <t>Injured</t>
+  </si>
+  <si>
+    <t>B/F</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Short Run</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>Shoulders</t>
+  </si>
+  <si>
+    <t>BW Exercises</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -175,19 +182,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,49 +507,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ADBCD0-968F-469A-8B27-8E7CAEBDE06E}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="14.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>21</v>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -556,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1">
         <v>30</v>
@@ -581,6 +584,9 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -590,7 +596,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>90</v>
@@ -610,7 +616,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1">
         <v>120</v>
@@ -630,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1">
         <v>30</v>
@@ -653,7 +659,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
         <v>36</v>
@@ -675,6 +681,12 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -684,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1">
         <v>30</v>
@@ -707,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1">
         <v>90</v>
@@ -726,6 +738,12 @@
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -735,7 +753,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1">
         <v>40</v>
@@ -750,7 +768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45217</v>
       </c>
@@ -758,7 +776,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1">
         <v>90</v>
@@ -775,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
         <v>40</v>
@@ -798,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1">
         <v>90</v>
@@ -817,6 +835,12 @@
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -826,7 +850,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1">
         <v>34</v>
@@ -849,7 +873,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1">
         <v>90</v>
@@ -869,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1">
         <v>40</v>
@@ -895,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1">
         <v>60</v>
@@ -914,6 +938,12 @@
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -923,7 +953,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1">
         <v>40</v>
@@ -946,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D23" s="1">
         <v>30</v>
@@ -969,7 +999,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D24" s="1">
         <v>70</v>
@@ -988,16 +1018,22 @@
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45227</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D26" s="1">
         <v>35</v>
@@ -1020,7 +1056,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1">
         <v>90</v>
@@ -1033,14 +1069,14 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>25</v>
+      <c r="A28" s="2">
+        <v>45228</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" s="1">
         <v>90</v>
@@ -1057,7 +1093,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D29" s="1">
         <v>30</v>
@@ -1080,7 +1116,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D30" s="1">
         <v>80</v>
@@ -1103,7 +1139,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D31" s="1">
         <v>30</v>
@@ -1126,7 +1162,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D32" s="1">
         <v>90</v>
@@ -1145,6 +1181,12 @@
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -1154,7 +1196,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D34" s="1">
         <v>35</v>
@@ -1176,6 +1218,12 @@
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -1185,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D36" s="1">
         <v>45</v>
@@ -1208,7 +1256,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1">
         <v>120</v>
@@ -1228,7 +1276,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D38" s="1">
         <v>90</v>
@@ -1248,7 +1296,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D39" s="1">
         <v>35</v>
@@ -1268,10 +1316,10 @@
         <v>45236</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1">
         <v>10</v>
@@ -1291,7 +1339,7 @@
         <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D41" s="1">
         <v>75</v>
@@ -1311,7 +1359,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D42" s="1">
         <v>30</v>
@@ -1332,6 +1380,817 @@
       </c>
       <c r="B43" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>45240</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="1">
+        <v>90</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G44" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>45241</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45242</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45243</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="1">
+        <v>30</v>
+      </c>
+      <c r="E47" s="1">
+        <v>600</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="G47" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>45244</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="1">
+        <v>40</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="G48" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>45245</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="1">
+        <v>30</v>
+      </c>
+      <c r="E49" s="1">
+        <v>750</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="G49" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>45246</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="1">
+        <v>25</v>
+      </c>
+      <c r="E50" s="1">
+        <v>550</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.34166666666666662</v>
+      </c>
+      <c r="G50" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>45247</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1">
+        <v>110</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="G51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>45248</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" s="1">
+        <v>105</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.74444444444444446</v>
+      </c>
+      <c r="G52" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>45249</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>45250</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="1">
+        <v>32</v>
+      </c>
+      <c r="E54" s="1">
+        <v>750</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="G54" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>45251</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="1">
+        <v>44</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="G55" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>45252</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>45253</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="1">
+        <v>30</v>
+      </c>
+      <c r="E57" s="1">
+        <v>600</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="G57" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>45253</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="1">
+        <v>90</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G58" s="1">
+        <v>6</v>
+      </c>
+      <c r="H58" s="1">
+        <v>75.400000000000006</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>45254</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>45255</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D60" s="1">
+        <v>90</v>
+      </c>
+      <c r="G60" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>45256</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="1">
+        <v>120</v>
+      </c>
+      <c r="G61" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="1">
+        <v>30</v>
+      </c>
+      <c r="E62" s="1">
+        <v>700</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G62" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>45258</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="1">
+        <v>30</v>
+      </c>
+      <c r="E63" s="1">
+        <v>600</v>
+      </c>
+      <c r="F63" s="3">
+        <v>0.34513888888888888</v>
+      </c>
+      <c r="G63" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>45258</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>45259</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>45260</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="1">
+        <v>20</v>
+      </c>
+      <c r="E66" s="1">
+        <v>500</v>
+      </c>
+      <c r="F66" s="3">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="G66" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>45261</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>45262</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>45263</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>45264</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>45265</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>45266</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>45267</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>45268</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>45269</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>45270</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>45271</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="1">
+        <v>40</v>
+      </c>
+      <c r="F77" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G77" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>45272</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>45273</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>45274</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>45275</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>45276</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D82" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>45277</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>45278</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>45279</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D85" s="1">
+        <v>75</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G85" s="1">
+        <v>8</v>
+      </c>
+      <c r="H85" s="1">
+        <v>75.8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>45280</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>45281</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>45282</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>45283</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D89" s="1">
+        <v>15</v>
+      </c>
+      <c r="F89" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>45284</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D90" s="1">
+        <v>15</v>
+      </c>
+      <c r="F90" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="H90" s="1">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated exercis records with injury period
</commit_message>
<xml_diff>
--- a/Data/Records.xlsx
+++ b/Data/Records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohin\Transition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC6405B-ACD5-4D25-A70C-5399C3BE2802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430A7E02-8460-4CFD-B41C-8EF5F66E906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="26910" windowHeight="12990" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
+    <workbookView xWindow="4848" yWindow="1818" windowWidth="17280" windowHeight="9054" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,18 @@
   </si>
   <si>
     <t>BW Exercises</t>
+  </si>
+  <si>
+    <t>Stretching</t>
+  </si>
+  <si>
+    <t>Walking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walking </t>
+  </si>
+  <si>
+    <t>Cardio</t>
   </si>
 </sst>
 </file>
@@ -507,25 +519,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ADBCD0-968F-469A-8B27-8E7CAEBDE06E}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.15625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.15625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.15625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>45208</v>
       </c>
@@ -577,7 +589,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>45209</v>
       </c>
@@ -588,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>45210</v>
       </c>
@@ -608,7 +620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>45211</v>
       </c>
@@ -628,7 +640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>45212</v>
       </c>
@@ -651,7 +663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>45213</v>
       </c>
@@ -674,7 +686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>45214</v>
       </c>
@@ -688,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>45215</v>
       </c>
@@ -711,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>45215</v>
       </c>
@@ -731,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>45216</v>
       </c>
@@ -745,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>45217</v>
       </c>
@@ -768,7 +780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>45217</v>
       </c>
@@ -785,7 +797,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>45218</v>
       </c>
@@ -808,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>45218</v>
       </c>
@@ -828,7 +840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>45219</v>
       </c>
@@ -842,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
         <v>45220</v>
       </c>
@@ -865,7 +877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2">
         <v>45221</v>
       </c>
@@ -885,7 +897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2">
         <v>45222</v>
       </c>
@@ -911,7 +923,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2">
         <v>45222</v>
       </c>
@@ -931,7 +943,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2">
         <v>45223</v>
       </c>
@@ -945,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2">
         <v>45224</v>
       </c>
@@ -968,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2">
         <v>45225</v>
       </c>
@@ -991,7 +1003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2">
         <v>45225</v>
       </c>
@@ -1011,7 +1023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2">
         <v>45226</v>
       </c>
@@ -1025,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2">
         <v>45227</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2">
         <v>45227</v>
       </c>
@@ -1068,7 +1080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2">
         <v>45228</v>
       </c>
@@ -1085,7 +1097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2">
         <v>45229</v>
       </c>
@@ -1108,7 +1120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2">
         <v>45229</v>
       </c>
@@ -1131,7 +1143,7 @@
         <v>74.900000000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2">
         <v>45230</v>
       </c>
@@ -1154,7 +1166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2">
         <v>45230</v>
       </c>
@@ -1174,7 +1186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2">
         <v>45231</v>
       </c>
@@ -1188,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2">
         <v>45232</v>
       </c>
@@ -1211,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2">
         <v>45233</v>
       </c>
@@ -1225,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2">
         <v>45234</v>
       </c>
@@ -1248,7 +1260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2">
         <v>45234</v>
       </c>
@@ -1268,7 +1280,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2">
         <v>45235</v>
       </c>
@@ -1288,7 +1300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
         <v>45236</v>
       </c>
@@ -1311,7 +1323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2">
         <v>45236</v>
       </c>
@@ -1331,7 +1343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
         <v>45237</v>
       </c>
@@ -1351,7 +1363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2">
         <v>45238</v>
       </c>
@@ -1374,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2">
         <v>45239</v>
       </c>
@@ -1388,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2">
         <v>45240</v>
       </c>
@@ -1408,7 +1420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
         <v>45241</v>
       </c>
@@ -1422,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2">
         <v>45242</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2">
         <v>45243</v>
       </c>
@@ -1459,7 +1471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2">
         <v>45244</v>
       </c>
@@ -1482,7 +1494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2">
         <v>45245</v>
       </c>
@@ -1505,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2">
         <v>45246</v>
       </c>
@@ -1528,7 +1540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2">
         <v>45247</v>
       </c>
@@ -1548,7 +1560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2">
         <v>45248</v>
       </c>
@@ -1568,7 +1580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2">
         <v>45249</v>
       </c>
@@ -1582,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2">
         <v>45250</v>
       </c>
@@ -1605,7 +1617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2">
         <v>45251</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2">
         <v>45252</v>
       </c>
@@ -1642,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2">
         <v>45253</v>
       </c>
@@ -1665,7 +1677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2">
         <v>45253</v>
       </c>
@@ -1688,7 +1700,7 @@
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2">
         <v>45254</v>
       </c>
@@ -1702,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2">
         <v>45255</v>
       </c>
@@ -1719,7 +1731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2">
         <v>45256</v>
       </c>
@@ -1736,7 +1748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2">
         <v>45257</v>
       </c>
@@ -1759,7 +1771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2">
         <v>45258</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2">
         <v>45258</v>
       </c>
@@ -1796,7 +1808,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2">
         <v>45259</v>
       </c>
@@ -1810,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2">
         <v>45260</v>
       </c>
@@ -1833,7 +1845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2">
         <v>45261</v>
       </c>
@@ -1847,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2">
         <v>45262</v>
       </c>
@@ -1861,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2">
         <v>45263</v>
       </c>
@@ -1875,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2">
         <v>45264</v>
       </c>
@@ -1889,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2">
         <v>45265</v>
       </c>
@@ -1903,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2">
         <v>45266</v>
       </c>
@@ -1917,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2">
         <v>45267</v>
       </c>
@@ -1931,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2">
         <v>45268</v>
       </c>
@@ -1945,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2">
         <v>45269</v>
       </c>
@@ -1959,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="2">
         <v>45270</v>
       </c>
@@ -1973,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="2">
         <v>45271</v>
       </c>
@@ -1993,7 +2005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2">
         <v>45272</v>
       </c>
@@ -2007,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="2">
         <v>45273</v>
       </c>
@@ -2021,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="2">
         <v>45274</v>
       </c>
@@ -2035,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="2">
         <v>45275</v>
       </c>
@@ -2049,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="2">
         <v>45276</v>
       </c>
@@ -2063,7 +2075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="2">
         <v>45277</v>
       </c>
@@ -2077,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="2">
         <v>45278</v>
       </c>
@@ -2091,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="2">
         <v>45279</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="2">
         <v>45280</v>
       </c>
@@ -2128,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="2">
         <v>45281</v>
       </c>
@@ -2142,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2">
         <v>45282</v>
       </c>
@@ -2156,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="2">
         <v>45283</v>
       </c>
@@ -2173,7 +2185,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="2">
         <v>45284</v>
       </c>
@@ -2191,6 +2203,368 @@
       </c>
       <c r="H90" s="1">
         <v>75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="2">
+        <v>45285</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="2">
+        <v>45286</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="2">
+        <v>45287</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="2">
+        <v>45288</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D94" s="1">
+        <v>10</v>
+      </c>
+      <c r="F94" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="2">
+        <v>45289</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D95" s="1">
+        <v>10</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="2">
+        <v>45290</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D97" s="1">
+        <v>15</v>
+      </c>
+      <c r="F97" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="2">
+        <v>45292</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D98" s="1">
+        <v>25</v>
+      </c>
+      <c r="F98" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="2">
+        <v>45293</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="2">
+        <v>45294</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="2">
+        <v>45295</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="2">
+        <v>45296</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="2">
+        <v>45297</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="2">
+        <v>45298</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="2">
+        <v>45299</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D105" s="1">
+        <v>30</v>
+      </c>
+      <c r="F105" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G105" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D106" s="1">
+        <v>30</v>
+      </c>
+      <c r="F106" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G106" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D107" s="1">
+        <v>30</v>
+      </c>
+      <c r="F107" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="G107" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="2">
+        <v>45302</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D108" s="1">
+        <v>15</v>
+      </c>
+      <c r="F108" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G108" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="2">
+        <v>45303</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D109" s="1">
+        <v>30</v>
+      </c>
+      <c r="F109" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G109" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="2">
+        <v>45304</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D110" s="1">
+        <v>15</v>
+      </c>
+      <c r="F110" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G110" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="2">
+        <v>45305</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D111" s="1">
+        <v>30</v>
+      </c>
+      <c r="F111" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G111" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="2">
+        <v>45306</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dashboard to visualise data
</commit_message>
<xml_diff>
--- a/Data/Records.xlsx
+++ b/Data/Records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohin\Transition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430A7E02-8460-4CFD-B41C-8EF5F66E906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1F1168-90B8-49FA-A062-2372175DCEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4848" yWindow="1818" windowWidth="17280" windowHeight="9054" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{E4FFC638-7B22-4057-83A7-F5AF7C23B63E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -519,25 +519,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ADBCD0-968F-469A-8B27-8E7CAEBDE06E}">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.15625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.15625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.83984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.15625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45208</v>
       </c>
@@ -589,7 +589,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45209</v>
       </c>
@@ -600,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45210</v>
       </c>
@@ -620,7 +620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45211</v>
       </c>
@@ -640,7 +640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45212</v>
       </c>
@@ -663,7 +663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45213</v>
       </c>
@@ -686,7 +686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45214</v>
       </c>
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45215</v>
       </c>
@@ -723,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45215</v>
       </c>
@@ -743,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45216</v>
       </c>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45217</v>
       </c>
@@ -780,7 +780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45217</v>
       </c>
@@ -797,7 +797,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45218</v>
       </c>
@@ -820,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45218</v>
       </c>
@@ -840,7 +840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45219</v>
       </c>
@@ -854,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45220</v>
       </c>
@@ -877,7 +877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45221</v>
       </c>
@@ -897,7 +897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45222</v>
       </c>
@@ -923,7 +923,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45222</v>
       </c>
@@ -943,7 +943,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45223</v>
       </c>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45224</v>
       </c>
@@ -980,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45225</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45225</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45226</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45227</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45227</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45228</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45229</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45229</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>74.900000000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45230</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45230</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45231</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45232</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45233</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45234</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45234</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45235</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45236</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45236</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45237</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45238</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45239</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45240</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45241</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45242</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45243</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45244</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45245</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45246</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45247</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45248</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45249</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45250</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45251</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>45252</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>45253</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>45253</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>45254</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>45255</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>45256</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>45257</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>45258</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>45258</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>45259</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>45260</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>45261</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>45262</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>45263</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>45264</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>45265</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>45266</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>45267</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>45268</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>45269</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>45270</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>45271</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>45272</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>45273</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>45274</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>45275</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>45276</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>45277</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>45278</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>45279</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>45280</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>45281</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>45282</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>45283</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>45284</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>45285</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>45286</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>45287</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>45288</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>45289</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>45290</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>45291</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>45292</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>45293</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>45294</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>45295</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>45296</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>45297</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>45298</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>45299</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>45300</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>45301</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>45302</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>45303</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>45304</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>45305</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>45306</v>
       </c>
@@ -2564,6 +2564,237 @@
         <v>30</v>
       </c>
       <c r="D112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>45307</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D113" s="1">
+        <v>0</v>
+      </c>
+      <c r="F113" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="G113" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>45308</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D114" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>45309</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D115" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>45310</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D116" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>45311</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D117" s="1">
+        <v>15</v>
+      </c>
+      <c r="F117" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G117" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>45312</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>45313</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D119" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>45314</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D120" s="1">
+        <v>15</v>
+      </c>
+      <c r="F120" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>45315</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D121" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>45316</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D122" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>45317</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D123" s="1">
+        <v>15</v>
+      </c>
+      <c r="F123" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G123" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>45318</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D124" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>45319</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D125" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>45320</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>45321</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D127" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>